<commit_message>
Tweak Canterbury.mp for Suburbs Limit decimals in Unmatched.sql Correct extra 0 in CitySize
</commit_message>
<xml_diff>
--- a/scripts/Suburbs/Code/CitySize.xlsx
+++ b/scripts/Suburbs/Code/CitySize.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gct23\nzopengps\scripts\Suburbs\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9F0433-D9B8-482C-8B00-896B513587CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4486310F-D3CF-4454-ACF9-1B7D8528AE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23295" yWindow="1440" windowWidth="14040" windowHeight="12090" xr2:uid="{AFAC6D98-48B7-4468-98EF-0A58E991226C}"/>
+    <workbookView xWindow="-13920" yWindow="1185" windowWidth="18840" windowHeight="12555" xr2:uid="{AFAC6D98-48B7-4468-98EF-0A58E991226C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3566,14 +3566,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0400B7C0-E8D6-4738-81FE-227535C8F758}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="96.5703125" customWidth="1"/>
-    <col min="2" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.5703125" customWidth="1"/>
@@ -3690,8 +3691,8 @@
         <v>1000000</v>
       </c>
       <c r="O2" t="str">
-        <f>B2&amp;"00"</f>
-        <v>0x0100</v>
+        <f>SUBSTITUTE(B2,"0x0","0x")&amp;"00"</f>
+        <v>0x100</v>
       </c>
       <c r="P2">
         <f>K2*$N2</f>
@@ -3759,8 +3760,8 @@
         <v>1000000</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O18" si="10">B3&amp;"00"</f>
-        <v>0x0200</v>
+        <f t="shared" ref="O3:O18" si="10">SUBSTITUTE(B3,"0x0","0x")&amp;"00"</f>
+        <v>0x200</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P18" ca="1" si="11">K3*$N3</f>
@@ -3829,7 +3830,7 @@
       </c>
       <c r="O4" t="str">
         <f t="shared" si="10"/>
-        <v>0x0300</v>
+        <v>0x300</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="11"/>
@@ -3898,7 +3899,7 @@
       </c>
       <c r="O5" t="str">
         <f t="shared" si="10"/>
-        <v>0x0400</v>
+        <v>0x400</v>
       </c>
       <c r="P5">
         <f t="shared" ca="1" si="11"/>
@@ -3967,7 +3968,7 @@
       </c>
       <c r="O6" t="str">
         <f t="shared" si="10"/>
-        <v>0x0500</v>
+        <v>0x500</v>
       </c>
       <c r="P6">
         <f t="shared" ca="1" si="11"/>
@@ -4036,7 +4037,7 @@
       </c>
       <c r="O7" t="str">
         <f t="shared" si="10"/>
-        <v>0x0600</v>
+        <v>0x600</v>
       </c>
       <c r="P7">
         <f t="shared" ca="1" si="11"/>
@@ -4105,7 +4106,7 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" si="10"/>
-        <v>0x0700</v>
+        <v>0x700</v>
       </c>
       <c r="P8">
         <f t="shared" ca="1" si="11"/>
@@ -4174,7 +4175,7 @@
       </c>
       <c r="O9" t="str">
         <f t="shared" si="10"/>
-        <v>0x0800</v>
+        <v>0x800</v>
       </c>
       <c r="P9">
         <f t="shared" ca="1" si="11"/>
@@ -4243,7 +4244,7 @@
       </c>
       <c r="O10" t="str">
         <f t="shared" si="10"/>
-        <v>0x0900</v>
+        <v>0x900</v>
       </c>
       <c r="P10">
         <f t="shared" ca="1" si="11"/>
@@ -4312,7 +4313,7 @@
       </c>
       <c r="O11" t="str">
         <f t="shared" si="10"/>
-        <v>0x0a00</v>
+        <v>0xa00</v>
       </c>
       <c r="P11">
         <f t="shared" ca="1" si="11"/>
@@ -4381,7 +4382,7 @@
       </c>
       <c r="O12" t="str">
         <f t="shared" si="10"/>
-        <v>0x0b00</v>
+        <v>0xb00</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="11"/>
@@ -4450,7 +4451,7 @@
       </c>
       <c r="O13" t="str">
         <f t="shared" si="10"/>
-        <v>0x0c00</v>
+        <v>0xc00</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="11"/>
@@ -4519,7 +4520,7 @@
       </c>
       <c r="O14" t="str">
         <f t="shared" si="10"/>
-        <v>0x0d00</v>
+        <v>0xd00</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="11"/>
@@ -4588,7 +4589,7 @@
       </c>
       <c r="O15" t="str">
         <f t="shared" si="10"/>
-        <v>0x0e00</v>
+        <v>0xe00</v>
       </c>
       <c r="P15" s="3">
         <v>500</v>
@@ -4655,7 +4656,7 @@
       </c>
       <c r="O16" t="str">
         <f t="shared" si="10"/>
-        <v>0x0f00</v>
+        <v>0xf00</v>
       </c>
       <c r="P16">
         <f t="shared" si="11"/>

</xml_diff>